<commit_message>
Add products to cart
</commit_message>
<xml_diff>
--- a/Locators/amazon_locators.xlsx
+++ b/Locators/amazon_locators.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Locator_ids" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>css=div[id*='nav-logo']</t>
   </si>
@@ -68,6 +68,114 @@
   </si>
   <si>
     <t>Amazon_Sign_Out_Button_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//span[contains(text(),'Departments')])</t>
+  </si>
+  <si>
+    <t>Amazon_Electronics_Drop_Down_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//span[contains(text(),'Electronics')])</t>
+  </si>
+  <si>
+    <t>Amazon_Departments_Drop_Down_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//span[contains(text(),'Headphones')])</t>
+  </si>
+  <si>
+    <t>Amazon_Headphones_Drop_Down_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//a[contains(@class,'a-link-normal')]//img)[1]</t>
+  </si>
+  <si>
+    <t>Amazon_Headphones_First_Product_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//input[contains(@id,'add-to-cart-button')])[1]</t>
+  </si>
+  <si>
+    <t>xpath=(//a[contains(@class,'close-button')])</t>
+  </si>
+  <si>
+    <t>Amazon_Add_To_Cart_Button_xpath</t>
+  </si>
+  <si>
+    <t>Amazon_Cart_Close_Button_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//input[contains(@id,'searchtextbox')])</t>
+  </si>
+  <si>
+    <t>xpath=(//input[contains(@type,'submit')])[1]</t>
+  </si>
+  <si>
+    <t>Amazon_Search_Submit_Button_xpath</t>
+  </si>
+  <si>
+    <t>Amazon_Search_Text_Box_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//a[contains(@class,'a-link-normal')]//img)[2]</t>
+  </si>
+  <si>
+    <t>Amazon_Search_Second_Product_xpath</t>
+  </si>
+  <si>
+    <t>xpath=//div[contains(@id,'selectQuantity')]//span[@role]</t>
+  </si>
+  <si>
+    <t>Amazon_Product_Quantity_Drop_Down_xpath</t>
+  </si>
+  <si>
+    <t>xpath=//a[@id='quantity_1']</t>
+  </si>
+  <si>
+    <t>Amazon_Product_Quantity_2_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//a[contains(@id,'nav-cart')])</t>
+  </si>
+  <si>
+    <t>Amazon_Product_Cart_Link_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//span[contains(@class,'sc-product-title')])</t>
+  </si>
+  <si>
+    <t>Amazon_Product_Titles_Added_In_Cart_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//input[contains(@name,'submit.delete')])</t>
+  </si>
+  <si>
+    <t>Amazon_Product_Delete_Buttons_Added_In_Cart_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//select[contains(@name,'quantity')])[1]</t>
+  </si>
+  <si>
+    <t>Amazon_Cart_First_Product_Quantity_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//input[contains(@name,'proceedToCheckout')])</t>
+  </si>
+  <si>
+    <t>Amazon_Cart_Proceed_To_Checkout_Button_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//h1[contains(text(),'shipping address')])</t>
+  </si>
+  <si>
+    <t>Amazon_Checkout_Shipping_Address_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//h4[contains(text(),'Added to Cart')])[2]</t>
+  </si>
+  <si>
+    <t>Verify_Amazon_Added_To_Cart_Text_Message_xpath</t>
   </si>
 </sst>
 </file>
@@ -385,16 +493,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="74" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -443,6 +551,142 @@
       </c>
       <c r="B6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -453,10 +697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,6 +725,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add macbook and remove headphone from cart
</commit_message>
<xml_diff>
--- a/Locators/amazon_locators.xlsx
+++ b/Locators/amazon_locators.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Locator_ids" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>css=div[id*='nav-logo']</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Amazon_Search_Second_Product_xpath</t>
   </si>
   <si>
-    <t>xpath=//div[contains(@id,'selectQuantity')]//span[@role]</t>
-  </si>
-  <si>
     <t>Amazon_Product_Quantity_Drop_Down_xpath</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>xpath=(//select[contains(@name,'quantity')])[1]</t>
   </si>
   <si>
-    <t>Amazon_Cart_First_Product_Quantity_xpath</t>
-  </si>
-  <si>
     <t>xpath=(//input[contains(@name,'proceedToCheckout')])</t>
   </si>
   <si>
@@ -176,6 +170,18 @@
   </si>
   <si>
     <t>Verify_Amazon_Added_To_Cart_Text_Message_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//select[contains(@name,'quantity')])</t>
+  </si>
+  <si>
+    <t>Amazon_Cart_First_Product_Quantity_1_xpath</t>
+  </si>
+  <si>
+    <t>xpath=(//span[contains(@class,'sc-product-title')][contains(text(),'Headphones')])</t>
+  </si>
+  <si>
+    <t>Amazon_Product_Headphones_Titles_Added_In_Cart_xpath</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,66 +633,74 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -699,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -727,10 +741,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>